<commit_message>
Criando as planilhas Titular, Informes e Notas
</commit_message>
<xml_diff>
--- a/Organizador de Declaracao de IR.xlsx
+++ b/Organizador de Declaracao de IR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbnog\Cursos DIO\Bootcamp Santander Excel com IA\Organizador-de-Imposto-de-Renda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BC7F75-7AF8-4CF6-8B4D-842DEA7ED122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF62984-626B-4A5C-8E90-2D1CA0EC2C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{780D04D5-E74D-4EA5-B752-CAF7AF068D1B}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="TITULAR" sheetId="1" r:id="rId1"/>
     <sheet name="INFORMES" sheetId="2" r:id="rId2"/>
     <sheet name="NOTAS" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,9 +38,301 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
+  <si>
+    <t>1. DADOS DO TÍTULAR</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>FELIPE SKYWALKER NOBUNAGA</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>NASCIMENTO</t>
+  </si>
+  <si>
+    <t>TÍTULO DE ELEITOR</t>
+  </si>
+  <si>
+    <t>CÔNJUGE</t>
+  </si>
+  <si>
+    <t>Mia Goth</t>
+  </si>
+  <si>
+    <t>RUA</t>
+  </si>
+  <si>
+    <t>Rua Dos limoeiros. Ruan, - Nº 180</t>
+  </si>
+  <si>
+    <t>RUA ABREVIADA</t>
+  </si>
+  <si>
+    <t>Rua Dos limoeiros. R, - Nº 180</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>TELEFONE</t>
+  </si>
+  <si>
+    <t>CELULAR</t>
+  </si>
+  <si>
+    <t>E-MAIL</t>
+  </si>
+  <si>
+    <t>HOUVE ALTERAÇÕES DA ENTREGA ANTERIOR</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>DEPENDENTE CÔNJUGE</t>
+  </si>
+  <si>
+    <t>NÃO</t>
+  </si>
+  <si>
+    <t>RESIDENTE DO EXTERIOR</t>
+  </si>
+  <si>
+    <t>wbn@dio.me</t>
+  </si>
+  <si>
+    <t>2. INFORMES DE RENDIMENTOS BANCÁRIOS</t>
+  </si>
+  <si>
+    <t>Preencha os dados da sua pessoa física abaixo</t>
+  </si>
+  <si>
+    <t>Preencha com seus dados atuais de cada banco</t>
+  </si>
+  <si>
+    <t>BANCO</t>
+  </si>
+  <si>
+    <t>VALOR ATUAL</t>
+  </si>
+  <si>
+    <t>ANEXO 🖇️</t>
+  </si>
+  <si>
+    <t>1 - Banco do Brasil</t>
+  </si>
+  <si>
+    <t>102 - XP Investimentos CCTVM S.A.</t>
+  </si>
+  <si>
+    <t>104 - Caixa Econômica Federal</t>
+  </si>
+  <si>
+    <t>119 - Banco Western Union do Brasil</t>
+  </si>
+  <si>
+    <t>184 - Banco Itaú BBA S.A.</t>
+  </si>
+  <si>
+    <t>197 - Stone Pagamentos</t>
+  </si>
+  <si>
+    <t>208 - Banco BTG Pactual</t>
+  </si>
+  <si>
+    <t>212 - Banco Original</t>
+  </si>
+  <si>
+    <t>218 - Banco Bonsucesso</t>
+  </si>
+  <si>
+    <t>229 - Banco Cruzeiro do Sul</t>
+  </si>
+  <si>
+    <t>237 - Banco Bradesco</t>
+  </si>
+  <si>
+    <t>24 - Banco de Pernambuco</t>
+  </si>
+  <si>
+    <t>241 - Banco Clássico</t>
+  </si>
+  <si>
+    <t>250 - Banco de Crédito e Varejo (BCV)</t>
+  </si>
+  <si>
+    <t>260 - Nubank</t>
+  </si>
+  <si>
+    <t>29 - Banco do Estado do Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>290 - PagBank</t>
+  </si>
+  <si>
+    <t>3 - Banco da Amazônia</t>
+  </si>
+  <si>
+    <t>33 - Banco Santander</t>
+  </si>
+  <si>
+    <t>336 - C6 Bank</t>
+  </si>
+  <si>
+    <t>341 - Itaú Unibanco</t>
+  </si>
+  <si>
+    <t>37 - Banco do Estado do Pará</t>
+  </si>
+  <si>
+    <t>376 - Banco JPMorgan S.A.</t>
+  </si>
+  <si>
+    <t>380 - PicPay</t>
+  </si>
+  <si>
+    <t>4 - Banco do Nordeste do Brasil</t>
+  </si>
+  <si>
+    <t>41 - Banco do Estado do Rio Grande do Sul</t>
+  </si>
+  <si>
+    <t>422 - Banco Safra</t>
+  </si>
+  <si>
+    <t>44 - Banco BVA</t>
+  </si>
+  <si>
+    <t>464 - Banco Sumitomo Mitsui Brasileiro</t>
+  </si>
+  <si>
+    <t>477 - Citibank</t>
+  </si>
+  <si>
+    <t>600 - Banco Luso Brasileiro</t>
+  </si>
+  <si>
+    <t>604 - Banco Industrial do Brasil</t>
+  </si>
+  <si>
+    <t>610 - Banco VR</t>
+  </si>
+  <si>
+    <t>62 - Hipercard Banco Múltiplo</t>
+  </si>
+  <si>
+    <t>634 - Banco Triângulo</t>
+  </si>
+  <si>
+    <t>65 - Banco Lemon</t>
+  </si>
+  <si>
+    <t>654 - Banco AJ Renner</t>
+  </si>
+  <si>
+    <t>655 - Banco Votorantim</t>
+  </si>
+  <si>
+    <t>66 - Banco Morgan Stanley</t>
+  </si>
+  <si>
+    <t>707 - Banco Daycoval</t>
+  </si>
+  <si>
+    <t>72 - Banco Rural Mais</t>
+  </si>
+  <si>
+    <t>734 - Banco Gerdau</t>
+  </si>
+  <si>
+    <t>735 - Banco Neon</t>
+  </si>
+  <si>
+    <t>74 - Banco J. Safra</t>
+  </si>
+  <si>
+    <t>746 - Banco Modal</t>
+  </si>
+  <si>
+    <t>748 - Banco Cooperativo Sicredi S.A.</t>
+  </si>
+  <si>
+    <t>749 - Banco Simples</t>
+  </si>
+  <si>
+    <t>77 - Banco Inter</t>
+  </si>
+  <si>
+    <t>79 - Banco JBS</t>
+  </si>
+  <si>
+    <t>82 - Banco Topázio</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t>1º Banco</t>
+  </si>
+  <si>
+    <t>2º Banco</t>
+  </si>
+  <si>
+    <t>3º Banco</t>
+  </si>
+  <si>
+    <t>iau_2025.pdf</t>
+  </si>
+  <si>
+    <t>santander_2025.pdf</t>
+  </si>
+  <si>
+    <t>c6bank_2025.pdf</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>3. NOTAS BANCÁRIAS OU EXTRATOS DE HOLERITES</t>
+  </si>
+  <si>
+    <t>São todos os valores de entrada mês a mês</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>HOLERITE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+    <numFmt numFmtId="165" formatCode="00000\-000"/>
+    <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;) &quot;0000&quot;-&quot;0000"/>
+    <numFmt numFmtId="167" formatCode="&quot;(&quot;00&quot;) &quot;00000&quot;-&quot;0000"/>
+    <numFmt numFmtId="170" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="173" formatCode="mmmm&quot;-&quot;yyyy"/>
+  </numFmts>
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -47,8 +340,103 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="0.89999084444715716"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,8 +449,31 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE37BF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -70,18 +481,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFEE37BF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFEE37BF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="170" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="9" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Neutro" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="173" formatCode="mmmm&quot;-&quot;yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -109,13 +706,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1400174</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -276,14 +873,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -363,14 +960,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -436,14 +1033,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -509,14 +1106,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -587,18 +1184,18 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1628775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -613,7 +1210,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="200025" y="3543300"/>
+          <a:off x="200025" y="3867150"/>
           <a:ext cx="1428750" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -642,18 +1239,18 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1104899</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -704,6 +1301,73 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Retângulo 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F632D27D-CAE6-4DEB-9E5F-1715BADDA563}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5429250" y="4152900"/>
+          <a:ext cx="2886075" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>PRÓXIMO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> -&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -713,14 +1377,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1400174</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -880,13 +1544,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -953,14 +1617,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1040,14 +1704,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1113,14 +1777,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1191,18 +1855,18 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1628775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1246,18 +1910,18 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1104899</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1308,6 +1972,135 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{814A8065-14F8-4201-9ACA-A3C97E959734}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5448300" y="4638675"/>
+          <a:ext cx="2886075" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>PRÓXIMO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> -&gt;</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2905125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo 9">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FD15E11-B22B-DD14-903F-94656AD46821}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495550" y="4638675"/>
+          <a:ext cx="2886075" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>&lt;- ANTERIOR</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1317,14 +2110,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1400174</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1484,14 +2277,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1557,14 +2350,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1630,14 +2423,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1747837</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1717,13 +2510,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1795,18 +2588,18 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1628775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1850,18 +2643,18 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1104899</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1912,7 +2705,81 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E6BD543-D284-4A23-9884-830DE7494C50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2486026" y="1019175"/>
+          <a:ext cx="1581150" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>&lt;- ANTERIOR</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA1FD1B3-0AE8-47A8-8AA9-7AB62E45BF2B}" name="Tabela2" displayName="Tabela2" ref="C8:E24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="C8:E24" xr:uid="{FA1FD1B3-0AE8-47A8-8AA9-7AB62E45BF2B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D67C023D-8076-4BF8-8FDF-92607E987116}" name="DATA" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0FD21263-3146-4C76-8EEB-9AF11E644DB6}" name="CATEGORIA" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0706E580-56FD-48D4-B277-1F5FDBC837E5}" name="VALOR" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2280,26 +3147,166 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5C50E2-830F-4BE9-A306-67BCC5537548}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6">
+        <v>12312312398</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
+        <v>34605</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>31713388</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8">
+        <v>987654321</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1131713388</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10">
+        <v>11931713388</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D19" xr:uid="{ED544CF2-D82E-41D4-8009-F99F4ABADA98}">
+      <formula1>"SIM,NÃO"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D16" r:id="rId1" xr:uid="{A3A51090-7165-4309-837A-68375D6676D6}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C49F7-335F-41F6-AE00-2C3428E92507}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1"/>
+  <dimension ref="A3:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -2308,17 +3315,149 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="3:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C6" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="16">
+        <f>SUM(D11,D16,D21)</f>
+        <v>5495882.1299999999</v>
+      </c>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13">
+        <v>546365.23</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1375147.36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3574369.54</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Banco não encontrado" error="Informe um banco da lista." promptTitle="Informe um banco" prompt="Informe um banco vinculado ao seu CPF." xr:uid="{A0296B67-0FDD-43D6-B89F-9BBB6480B3DC}">
+          <x14:formula1>
+            <xm:f>Tabelas!$A$2:$A$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>D10 D15 D20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDBE125-8E85-4AB1-A227-78E564D88ECA}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A3:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -2327,9 +3466,416 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C7" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C9" s="23">
+        <v>45811</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="22">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C11" s="23"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C12" s="23"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C13" s="23"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C14" s="23"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C15" s="23"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C16" s="23"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C17" s="23"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+    </row>
+    <row r="18" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="23"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C19" s="23"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C20" s="23"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+    </row>
+    <row r="21" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C21" s="23"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C22" s="23"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C23" s="23"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C24" s="23"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C7:E7"/>
+  </mergeCells>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D24" xr:uid="{DAF45730-84DE-48CC-B94F-CF3493372FF7}">
+      <formula1>"HOLERITE,CNPJ,FREELANCE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A5C479-B81C-4A9F-BAE6-8D09A5CC5554}">
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Protegendo as planilhas deixando liberado somente onde há entrada de dados
</commit_message>
<xml_diff>
--- a/Organizador de Declaracao de IR.xlsx
+++ b/Organizador de Declaracao de IR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wbnog\Cursos DIO\Bootcamp Santander Excel com IA\Organizador-de-Imposto-de-Renda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF62984-626B-4A5C-8E90-2D1CA0EC2C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E85996E-2FE9-4934-AA33-768F72DE2BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{780D04D5-E74D-4EA5-B752-CAF7AF068D1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="0" xr2:uid="{780D04D5-E74D-4EA5-B752-CAF7AF068D1B}"/>
   </bookViews>
   <sheets>
     <sheet name="TITULAR" sheetId="1" r:id="rId1"/>
@@ -329,8 +329,8 @@
     <numFmt numFmtId="165" formatCode="00000\-000"/>
     <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;) &quot;0000&quot;-&quot;0000"/>
     <numFmt numFmtId="167" formatCode="&quot;(&quot;00&quot;) &quot;00000&quot;-&quot;0000"/>
-    <numFmt numFmtId="170" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="173" formatCode="mmmm&quot;-&quot;yyyy"/>
+    <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="169" formatCode="mmmm&quot;-&quot;yyyy"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -526,7 +526,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -562,36 +562,51 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="9" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -601,21 +616,6 @@
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
   <dxfs count="5">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="173" formatCode="mmmm&quot;-&quot;yyyy"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -644,6 +644,21 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="mmmm&quot;-&quot;yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -2774,9 +2789,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA1FD1B3-0AE8-47A8-8AA9-7AB62E45BF2B}" name="Tabela2" displayName="Tabela2" ref="C8:E24" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="C8:E24" xr:uid="{FA1FD1B3-0AE8-47A8-8AA9-7AB62E45BF2B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D67C023D-8076-4BF8-8FDF-92607E987116}" name="DATA" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{0FD21263-3146-4C76-8EEB-9AF11E644DB6}" name="CATEGORIA" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{0706E580-56FD-48D4-B277-1F5FDBC837E5}" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D67C023D-8076-4BF8-8FDF-92607E987116}" name="DATA" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0FD21263-3146-4C76-8EEB-9AF11E644DB6}" name="CATEGORIA" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0706E580-56FD-48D4-B277-1F5FDBC837E5}" name="VALOR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3149,7 +3164,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A3:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3168,11 +3183,11 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
@@ -3287,10 +3302,11 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:E4"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D19" xr:uid="{ED544CF2-D82E-41D4-8009-F99F4ABADA98}">
       <formula1>"SIM,NÃO"</formula1>
     </dataValidation>
@@ -3306,10 +3322,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9C49F7-335F-41F6-AE00-2C3428E92507}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A3:E22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
+      <extLst>
+        <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
+          <xlsdti:showDataTypeIcons visible="0"/>
+        </ext>
+      </extLst>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3319,6 +3340,9 @@
     <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="24"/>
+    </row>
     <row r="3" spans="3:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>22</v>
@@ -3327,26 +3351,26 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="16">
+      <c r="C7" s="21">
         <f>SUM(D11,D16,D21)</f>
         <v>5495882.1299999999</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="22"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3362,7 +3386,7 @@
       <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>546365.23</v>
       </c>
     </row>
@@ -3375,7 +3399,7 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3391,7 +3415,7 @@
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <v>1375147.36</v>
       </c>
     </row>
@@ -3404,7 +3428,7 @@
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3420,7 +3444,7 @@
       <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <v>3574369.54</v>
       </c>
     </row>
@@ -3433,6 +3457,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:D7"/>
@@ -3459,8 +3484,13 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A3:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+      <extLst>
+        <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
+          <xlsdti:showDataTypeIcons visible="0"/>
+        </ext>
+      </extLst>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3479,122 +3509,123 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="23">
+      <c r="C9" s="25">
         <v>45811</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="27">
         <v>8000</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="23"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="23"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
     </row>
     <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C12" s="23"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C13" s="23"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C14" s="23"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C15" s="23"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C16" s="23"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C17" s="23"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C18" s="23"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
     </row>
     <row r="19" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C19" s="23"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C20" s="23"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C21" s="23"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C22" s="23"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
     </row>
     <row r="23" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C23" s="23"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C24" s="23"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D24" xr:uid="{DAF45730-84DE-48CC-B94F-CF3493372FF7}">
       <formula1>"HOLERITE,CNPJ,FREELANCE"</formula1>
     </dataValidation>
@@ -3621,7 +3652,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>